<commit_message>
Add units of sale and cost per unit analysis with enhanced visualizations
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,93 +440,180 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Units of Sale</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cost per Unit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="n">
+        <v>45974</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Laptops</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>45000</v>
       </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9000</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Smartphones</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>67000</v>
       </c>
+      <c r="D3" t="n">
+        <v>25</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2680</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Tablets</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>32000</v>
       </c>
+      <c r="D4" t="n">
+        <v>18</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1777.78</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="n">
+        <v>45985</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Monitors</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>28000</v>
       </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2333.33</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="n">
+        <v>46033</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Keyboards</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>15000</v>
       </c>
+      <c r="D6" t="n">
+        <v>45</v>
+      </c>
+      <c r="E6" t="n">
+        <v>333.33</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="n">
+        <v>46040</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Mice</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>12000</v>
       </c>
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" t="n">
+        <v>240</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="n">
+        <v>46048</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Headphones</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>23000</v>
       </c>
+      <c r="D8" t="n">
+        <v>32</v>
+      </c>
+      <c r="E8" t="n">
+        <v>718.75</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="n">
+        <v>46053</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Webcams</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>18000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>642.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>